<commit_message>
update connection to DB
</commit_message>
<xml_diff>
--- a/Connect_DB.xlsx
+++ b/Connect_DB.xlsx
@@ -2,17 +2,18 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\mvc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\C# ASP.NET\QLNS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11730"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11730" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Xóa chuỗi kết nối cũ" sheetId="2" r:id="rId1"/>
+    <sheet name="Tạo kết nối mới" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -98,6 +99,87 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>103818</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>94268</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="981075" y="238125"/>
+          <a:ext cx="7657143" cy="7857143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>52834</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>87351</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9196834" y="600075"/>
+          <a:ext cx="14664917" cy="6781800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1004,9 +1086,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>

</xml_diff>